<commit_message>
Daftar Test Commit 2
</commit_message>
<xml_diff>
--- a/Daftar Akun.xlsx
+++ b/Daftar Akun.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -99,6 +99,69 @@
   </si>
   <si>
     <t>applicationtester77@gmail.com</t>
+  </si>
+  <si>
+    <t>nopol</t>
+  </si>
+  <si>
+    <t>kontrak</t>
+  </si>
+  <si>
+    <t>belum</t>
+  </si>
+  <si>
+    <t>sudah</t>
+  </si>
+  <si>
+    <t>noPolEmpty</t>
+  </si>
+  <si>
+    <t>noPolNotFound</t>
+  </si>
+  <si>
+    <t>Aing Macan</t>
+  </si>
+  <si>
+    <t>Aing Singa</t>
+  </si>
+  <si>
+    <t>Aing Gajah</t>
+  </si>
+  <si>
+    <t>phoneNoEmpty</t>
+  </si>
+  <si>
+    <t>phoneNoShort</t>
+  </si>
+  <si>
+    <t>phoneNoExist</t>
+  </si>
+  <si>
+    <t>passInvalid</t>
+  </si>
+  <si>
+    <t>confPassNotMatch</t>
+  </si>
+  <si>
+    <t>Tikus</t>
+  </si>
+  <si>
+    <t>Jerapah</t>
+  </si>
+  <si>
+    <t>Application2!</t>
+  </si>
+  <si>
+    <t>Yahoo</t>
+  </si>
+  <si>
+    <t>succeed</t>
+  </si>
+  <si>
+    <t>w1316pk</t>
+  </si>
+  <si>
+    <t>application</t>
   </si>
 </sst>
 </file>
@@ -427,23 +490,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +535,14 @@
       <c r="I1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -488,14 +558,20 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
+      <c r="G2">
+        <v>261294</v>
+      </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -514,14 +590,20 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
+      <c r="G3">
+        <v>261294</v>
+      </c>
       <c r="H3" t="s">
         <v>11</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -538,14 +620,20 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
+      <c r="G4">
+        <v>261294</v>
+      </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -564,14 +652,20 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
+      <c r="G5">
+        <v>261294</v>
+      </c>
       <c r="H5" t="s">
         <v>18</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -590,11 +684,258 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
+      <c r="G6">
+        <v>261294</v>
+      </c>
       <c r="H6" t="s">
         <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>261294</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>822</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>261294</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>82297476950</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>261294</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>82297476950</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>261294</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>82297476950</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>261294</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>82297476950</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>261294</v>
+      </c>
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>261294</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>261294</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -602,6 +943,14 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>